<commit_message>
cambio en el main
</commit_message>
<xml_diff>
--- a/resources/datos.xlsx
+++ b/resources/datos.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="16">
   <si>
     <t>persona</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t>www.google.com</t>
+  </si>
+  <si>
+    <t>Steve Wozniak</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>789789987</t>
+  </si>
+  <si>
+    <t>www.microsoft.com</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>www.apple.com</t>
   </si>
 </sst>
 </file>
@@ -415,7 +433,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C086D438-89EC-437E-800B-092276E422F5}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -659,6 +677,108 @@
         <v>9</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-4.7648109E8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="n">
+        <v>6.5037178E7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="n">
+        <v>6.5037178E7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-4.7648109E8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-1.94623651E9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="n">
+        <v>6.5037178E7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
añadido metodo anadir Trabajador a empresa
</commit_message>
<xml_diff>
--- a/resources/datos.xlsx
+++ b/resources/datos.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="16">
   <si>
     <t>persona</t>
   </si>
@@ -552,7 +552,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0</v>
+        <v>6.5037178E7</v>
       </c>
       <c r="E8" t="s">
         <v>3</v>
@@ -560,53 +560,53 @@
     </row>
     <row r="8">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D9" t="n">
-        <v>-4.7648109E8</v>
+        <v>6.5037178E7</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D10" t="n">
         <v>-4.7648109E8</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0</v>
+        <v>-1.94623651E9</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -614,152 +614,152 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D12" t="n">
-        <v>-4.7648109E8</v>
+        <v>6.5037178E7</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D13" t="n">
         <v>-4.7648109E8</v>
       </c>
       <c r="E13" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0</v>
+        <v>-4.7648109E8</v>
       </c>
       <c r="E14" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="n">
-        <v>-4.7648109E8</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-4.7648109E8</v>
+      </c>
+      <c r="E15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-4.7648109E8</v>
-      </c>
-      <c r="E15" t="s">
-        <v>3</v>
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-4.7648109E8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="n">
-        <v>6.5037178E7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>3</v>
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-4.7648109E8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="n">
-        <v>6.5037178E7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>3</v>
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-4.7648109E8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="n">
-        <v>-4.7648109E8</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-4.7648109E8</v>
+      </c>
+      <c r="E19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" t="n">
-        <v>-1.94623651E9</v>
-      </c>
-      <c r="E19" t="s">
-        <v>13</v>
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-4.7648109E8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="20">
@@ -767,16 +767,16 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D20" t="n">
-        <v>6.5037178E7</v>
+        <v>-4.7648109E8</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificaciones de jajcoco para cloudflare
</commit_message>
<xml_diff>
--- a/resources/datos.xlsx
+++ b/resources/datos.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="16">
   <si>
     <t>persona</t>
   </si>
@@ -444,13 +444,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>-4.7648109E8</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -458,36 +458,36 @@
     </row>
     <row r="2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>-4.7648109E8</v>
+        <v>0.0</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n">
         <v>-4.7648109E8</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -495,13 +495,13 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0</v>
+        <v>-4.7648109E8</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -509,19 +509,19 @@
     </row>
     <row r="5">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>-4.7648109E8</v>
+        <v>6.5037178E7</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -529,13 +529,13 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
-        <v>-4.7648109E8</v>
+        <v>6.5037178E7</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -543,36 +543,36 @@
     </row>
     <row r="7">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>6.5037178E7</v>
+        <v>-4.7648109E8</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D9" t="n">
-        <v>6.5037178E7</v>
+        <v>-1.94623651E9</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -580,16 +580,16 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D10" t="n">
-        <v>-4.7648109E8</v>
+        <v>6.5037178E7</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
@@ -597,16 +597,16 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.94623651E9</v>
+        <v>-4.7648109E8</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -614,16 +614,16 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D12" t="n">
-        <v>6.5037178E7</v>
+        <v>-4.7648109E8</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">

</xml_diff>